<commit_message>
Les sites E-commerces vendent prsque les mêmes produits , mais n'utilise pas les mêmes balises ou autres... Donc pour l'instant, j'ai reussi a recuperer les produit de Jumia de la categoy fashion Mode Je vais integrer selenium plus tard pour naviguer dans les differents pages su site.
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="ProduitJumia" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="produit Expat" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="ProduitJumia" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,203 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Nom</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Prix Produit</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Prix Promo</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Lunette Dior homme</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>75000.00</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Berlutti</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>125000.00</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Montre connectée originale</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>35000.00</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Montre femme de classe</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>25000.00</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Tondeuse HTC rechargeable</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>15000.00</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Galaxy watch 4 mémoire 16Go</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>140000.00</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Magic Plate - Block avec Plusieurs Formes pour enfant DIY</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>4000.00</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Mini Drone Mirage avec appareil photo pour enregistrement</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>16900.00</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Kangourou enfants</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Transats enfants</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,7 +728,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2 700 FCFA - 3 100 FCFA</t>
+          <t>2 700 FCFA</t>
         </is>
       </c>
     </row>
@@ -555,29 +752,29 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2022 Hommes Classic Martin Boots Running Baskets - Noir/Blanc</t>
+          <t>homme sport veste Ensemble  + pantalon 2 pièces -bleu foncé</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>18 798 FCFA</t>
+          <t>14 902 FCFA</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>8 699 FCFA</t>
+          <t>6 900 FCFA</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>homme sport veste Ensemble  + pantalon 2 pièces -bleu foncé</t>
+          <t>Baskets Décontractées pour Homme - Gris</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>14 902 FCFA</t>
+          <t>15 000 FCFA</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -589,394 +786,390 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Baskets Décontractées pour Homme - Gris</t>
+          <t>Pantalons Chino pour Homme-Noir</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>15 000 FCFA</t>
+          <t>5 990 FCFA</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>6 900 FCFA - 7 900 FCFA</t>
+          <t>3 900 FCFA</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Pantalons Chino pour Homme-Noir</t>
+          <t>Baskets à Lacets Respirants pour Hommes de Couleur Unie Basket de mode</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>5 990 FCFA</t>
+          <t>12 745 FCFA</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>3 900 FCFA</t>
+          <t>6 500 FCFA</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Baskets à Lacets Respirants pour Hommes de Couleur Unie Basket de mode</t>
+          <t>Chaussures Décontractées pour Hommes en simili cuir - Noir</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>12 745 FCFA</t>
+          <t>8 431 FCFA</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>6 500 FCFA - 6 900 FCFA</t>
+          <t>4 300 FCFA</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Chaussures Décontractées pour Hommes en simili cuir - Noir</t>
+          <t>Talons Hauts Sandales Chaussures Habillées</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>8 431 FCFA</t>
+          <t>8 834 FCFA</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>4 300 FCFA</t>
+          <t>4 990 FCFA</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Talons Hauts Sandales Chaussures Habillées</t>
+          <t>Baskets Décontractées Basses Pour Hommes - Blanc</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>8 834 FCFA</t>
+          <t>10 998 FCFA</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>4 990 FCFA</t>
+          <t>6 980 FCFA</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Baskets Décontractées Basses Pour Hommes - Blanc</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>10 998 FCFA</t>
-        </is>
-      </c>
+          <t>Montre F-200W-1ADF, bracelet en plastique, étanche, avec lumière LED</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
-          <t>6 980 FCFA</t>
+          <t>22 000 FCFA</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Montre F-200W-1ADF, bracelet en plastique, étanche, avec lumière LED</t>
+          <t>Collant en Coton - Bleu</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
-          <t>22 000 FCFA</t>
+          <t>15 000 FCFA</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Collant en Coton - Bleu</t>
+          <t>Zipper Hoodie Suit Hommes Femmes Sets Survêtement Pantalon Long 2 Pièces Costume</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>15 000 FCFA</t>
+          <t>22 150 FCFA - 22 170 FCFA</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>10 900 FCFA</t>
+          <t>11 890 FCFA - 14 920 FCFA</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Zipper Hoodie Suit Hommes Femmes Sets Survêtement Pantalon Long 2 Pièces Costume</t>
+          <t>Chemise à Capuche à Carreaux - Jaune</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>22 150 FCFA - 22 170 FCFA</t>
+          <t>12 998 FCFA</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>11 890 FCFA - 14 920 FCFA</t>
+          <t>8 900 FCFA</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Chemise à Capuche à Carreaux - Jaune</t>
+          <t>SAI Sacs à Bandoulière, Porte-documents, Sacs à Main -marron</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>12 998 FCFA</t>
+          <t>11 990 FCFA</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>8 900 FCFA</t>
+          <t>6 900 FCFA</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>SAI Sacs à Bandoulière, Porte-documents, Sacs à Main -marron</t>
+          <t>Baskets à Lacets Respirants pour Hommes de Couleur Unie</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>11 990 FCFA</t>
+          <t>25 000 FCFA</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>6 900 FCFA</t>
+          <t>7 250 FCFA</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Baskets à Lacets Respirants pour Hommes de Couleur Unie</t>
+          <t>Lunettes de lecture photogray anti reflet</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>25 000 FCFA</t>
+          <t>8 500 FCFA</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>7 250 FCFA</t>
+          <t>6 800 FCFA</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Lunettes de lecture photogray anti reflet</t>
+          <t>Chaussures Plates Confortables Respirantes Classiques Pour Hommes Marron</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>8 500 FCFA</t>
+          <t>45 990 FCFA</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>6 800 FCFA</t>
+          <t>17 900 FCFA</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Chaussures Plates Confortables Respirantes Classiques Pour Hommes Marron</t>
+          <t>manche courte Polo d'été pour hommes d'affaires décontracté</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>45 990 FCFA</t>
+          <t>9 960 FCFA</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>17 900 FCFA</t>
+          <t>4 500 FCFA</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>manche courte Polo d'été pour hommes d'affaires décontracté</t>
+          <t>Chaussures Baskets Pour Femme - Noir</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>9 960 FCFA</t>
+          <t>9 214 FCFA - 9 608 FCFA</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>4 500 FCFA</t>
+          <t>4 699 FCFA - 4 899 FCFA</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Chaussures Baskets Pour Femme - Noir</t>
+          <t>Chaussures de sport décontractées pour hommes-noir</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>9 214 FCFA - 9 608 FCFA</t>
+          <t>7 200 FCFA</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>4 699 FCFA - 4 899 FCFA</t>
+          <t>2 650 FCFA</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Chaussures de sport décontractées pour hommes-noir</t>
+          <t>Baskets Décontractées pour Hommes Walking Cheap -Bleu</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>7 200 FCFA</t>
+          <t>15 000 FCFA</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2 900 FCFA</t>
+          <t>5 500 FCFA</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Baskets Décontractées pour Hommes Walking Cheap -Bleu</t>
+          <t>Chaussures de course décontractées pour hommes-marron</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>15 000 FCFA</t>
+          <t>8 625 FCFA</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>5 500 FCFA</t>
+          <t>3 899 FCFA</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Chaussures de course décontractées pour hommes-marron</t>
+          <t>Chaussures de confort à semelle souple pour hommes</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>8 625 FCFA</t>
+          <t>16 900 FCFA</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>4 399 FCFA</t>
+          <t>8 300 FCFA</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Chaussures de confort à semelle souple pour hommes</t>
+          <t>Baskets Décontractées Pour Hommes + chaussette</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16 900 FCFA</t>
+          <t>10 526 FCFA</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>8 300 FCFA</t>
+          <t>4 300 FCFA</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Baskets Décontractées Pour Hommes + chaussette</t>
+          <t>Baskets de sport décontractées pour hommes Tide Noir et blanc</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>10 526 FCFA</t>
+          <t>11 808 FCFA</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>4 300 FCFA</t>
+          <t>7 500 FCFA - 8 500 FCFA</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Baskets de sport décontractées pour hommes Tide Noir et blanc</t>
+          <t>Chaussures Baskets  Pour Femmes Noires</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>11 808 FCFA</t>
+          <t>5 984 FCFA</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>7 500 FCFA - 8 500 FCFA</t>
+          <t>2 990 FCFA</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Chaussures Baskets  Pour Femmes Noires</t>
+          <t>Martin Boots Men's Tooling All-match High-top Shoes-black</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>5 984 FCFA</t>
+          <t>12 000 FCFA</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>3 190 FCFA</t>
+          <t>7 850 FCFA</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Martin Boots Men's Tooling All-match High-top Shoes-black</t>
+          <t>Fashion Baskets De Sport Femme - bleu</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -986,748 +1179,697 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>7 850 FCFA</t>
+          <t>5 990 FCFA - 6 690 FCFA</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Fashion Baskets De Sport Femme - bleu</t>
+          <t>Baskets à Lacets Respirants pour Hommes de Couleur Unie</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>12 000 FCFA</t>
+          <t>8 235 FCFA</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>5 990 FCFA - 6 690 FCFA</t>
+          <t>4 950 FCFA</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Baskets à Lacets Respirants pour Hommes de Couleur Unie</t>
+          <t>2021 Chaussures De Sport Mode Pour Hommes - Blanc</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>8 235 FCFA</t>
+          <t>15 684 FCFA</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>4 950 FCFA</t>
+          <t>7 999 FCFA</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2021 Chaussures De Sport Mode Pour Hommes - Blanc</t>
+          <t>Chaussures pour hommes baskets mode nouveau décontracté extérieur chaussures à la mode course Sport léger respirant baskets</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>15 684 FCFA</t>
+          <t>7 784 FCFA - 11 137 FCFA</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>7 999 FCFA</t>
+          <t>3 590 FCFA - 3 990 FCFA</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Chaussures pour hommes baskets mode nouveau décontracté extérieur chaussures à la mode course Sport léger respirant baskets</t>
+          <t>Chaussures de sport pour hommes - Noir</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7 784 FCFA</t>
+          <t>12 900 FCFA</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>3 590 FCFA</t>
+          <t>8 290 FCFA - 8 900 FCFA</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Chaussures de sport pour hommes - Noir</t>
+          <t>Fashion 2022 Basket Class Pour Homme - En noir et blanc</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>12 900 FCFA</t>
+          <t>14 400 FCFA</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>8 290 FCFA - 8 900 FCFA</t>
+          <t>3 990 FCFA</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2022 Hommes Classic Martin Boots Running Baskets - Noir/Blanc</t>
+          <t>Hommes Sac Poitrine Sac Bandoulière Sac Bourse Portefeuille Messenger Sac À Bandoulière Sling Satchel</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>18 798 FCFA</t>
+          <t>7 000 FCFA</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>8 699 FCFA</t>
+          <t>3 990 FCFA</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Hommes Sac Poitrine Sac Bandoulière Sac Bourse Portefeuille Messenger Sac À Bandoulière Sling Satchel</t>
+          <t>Lisseur cheveux CREPUS - Peigne électrique chauffante</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>7 000 FCFA</t>
+          <t>10 000 FCFA</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>3 990 FCFA</t>
+          <t>8 500 FCFA</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Lisseur cheveux CREPUS - Peigne électrique chauffante</t>
+          <t>4 en 1 Sac à main femmes sac dames sac femme sac à bandoulière Messenger fronde portefeuille cartable</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>10 000 FCFA</t>
+          <t>7 647 FCFA</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>8 500 FCFA</t>
+          <t>4 900 FCFA</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>4 en 1 Sac à main femmes sac dames sac femme sac à bandoulière Messenger fronde portefeuille cartable</t>
+          <t>Sac à Dos Pour Hommes Sac à dos pour femmes Sac ordinateur portable à Trois Pièces</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>7 647 FCFA</t>
+          <t>11 297 FCFA</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>6 290 FCFA</t>
+          <t>5 900 FCFA</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Sac à Dos Pour Hommes Sac à dos pour femmes Sac ordinateur portable à Trois Pièces</t>
+          <t>Lunettes de soleil rétro polarisées - Noir</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>11 297 FCFA</t>
+          <t>4 000 FCFA</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>5 300 FCFA</t>
+          <t>2 200 FCFA</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Sac Transparent Brillant Sac à Bandoulière à Poignée Carrée</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>7 451 FCFA</t>
-        </is>
-      </c>
+          <t>Baskets Décontractées Pour Hommes</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr">
         <is>
-          <t>3 800 FCFA</t>
+          <t>8 600 FCFA</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Combinaison de bracelet de montre à quartz</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>7 431 FCFA</t>
-        </is>
-      </c>
+          <t>Montre A Quartz Pour Femme - Or</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr">
         <is>
-          <t>3 790 FCFA</t>
+          <t>1 450 FCFA</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Lunettes de soleil rétro polarisées - Noir</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>4 000 FCFA</t>
-        </is>
-      </c>
+          <t>Bijoux Ensemble Bracelet - 5 pièces</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2 200 FCFA</t>
+          <t>815 FCFA</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Pantalons De Survêtement Pour Hommes Respirant-Noir</t>
+          <t>Montre étanche d'affaires à double calendrier - Argent et or</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2 860 FCFA</t>
+          <t>5 900 FCFA</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Chemise décontractée à manches longues en lin pour hommes</t>
+          <t>4 Pièces - T-Shirt - Pour Homme - Noir, Noir, Gris, Blanc</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1 850 FCFA</t>
+          <t>3 290 FCFA</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Chemise à manches longues élégante à fleurs pour hommes</t>
+          <t>Men Faux Sac à Bandoulière En Cuir De Haute Qualité Mode Zipper Casual Bureau Sac Bandoulière</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr">
         <is>
-          <t>1 850 FCFA</t>
+          <t>3 995 FCFA</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Chaussures Habillées Pour Hommes</t>
+          <t>Chaussures Baskets Pour Homme Respirant - Noir</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr">
         <is>
-          <t>4 500 FCFA - 5 900 FCFA</t>
+          <t>2 135 FCFA</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Chemise à manches longues élégante à fleurs pour hommes</t>
+          <t>Portefeuille,Sac à dos,Sac à épaule,Sac De Messager Décontracté Oxford Pour Hommes</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr">
         <is>
-          <t>1 850 FCFA</t>
+          <t>2 400 FCFA</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>3 Pièces - T-Shirt - Pour Homme - Noir, Gris, Blanc</t>
+          <t>Coffret de priére de 6pcs - tapis de priere- parfum - Djalaba - chapelet - stylot - livre citadelle du musulmane</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2 700 FCFA</t>
+          <t>15 900 FCFA</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Chaussures De Sport Pour Hommes-noir</t>
+          <t>Sac de sport imperméable multifonctionnel sac à dos de remise en forme sac à main d'épaule de voyage/bagage</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2 320 FCFA</t>
+          <t>4 800 FCFA</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Chemise Hawaïenne imprimée Homme - multi</t>
+          <t>Lunettes De Soleil Vintage, Grand Cadre Carré, Métallisé Vintage, Unisexe De Haute Qualité</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr">
         <is>
-          <t>1 550 FCFA</t>
+          <t>4 020 FCFA</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Chaussures Habillées Pour Hommes</t>
+          <t>Chaussures De Sport Pour Hommes-noir</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr">
         <is>
-          <t>3 900 FCFA - 5 200 FCFA</t>
+          <t>2 320 FCFA</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Chemise Manches Longues Pour Homme-Bleu</t>
+          <t>T-shirt de couleur unie hommes en coton (6 t-shirts)</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2 740 FCFA</t>
+          <t>12 349 FCFA</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Montre à Quartz Pour Femme-d'or</t>
+          <t>Sac de taille tendance décontracté sac diagonal polyvalent sac de poitrine de voyage léger en plein air</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr">
         <is>
-          <t>1 265 FCFA</t>
+          <t>4 105 FCFA</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>4 Pièces - T-Shirt - Pour Homme - Noir, Noir, Gris, Blanc</t>
+          <t>Djellaba Marocaine A Manches Courtes - Rayure</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr">
         <is>
-          <t>3 290 FCFA</t>
+          <t>6 555 FCFA</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Sandale Compensée A Bandes Femme - Simili Cuir</t>
+          <t>Ensemble Djalaba pour homme - Djelaba + pantalon</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2 200 FCFA</t>
+          <t>9 999 FCFA</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Baskets Décontractées Pour Hommes + chaussette</t>
+          <t>Coffret de priére de 6pcs - tapis de priere- parfum - Djalaba - chapelet - stylo - livre citadelle du musulmane</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2 750 FCFA</t>
+          <t>16 900 FCFA</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Chemises à Manches Courtes Pour Hommes</t>
+          <t>Box de Luxe - 5 voiles Hijab en Satin</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr">
         <is>
-          <t>1 750 FCFA</t>
+          <t>13 500 FCFA</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Chaussures en Toile Homme Bleu + Ceinture</t>
+          <t>Pack de 5 Tee-shirt Col Rond en Coton qualité supérieur Manches Courtes</t>
         </is>
       </c>
       <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2 500 FCFA</t>
+          <t>9 499 FCFA</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Ensemble 2 Pièces Homme - T-shirt + Short Combinaisons De Sport Et De Loisirs</t>
+          <t>Pack Portefeuille Simili Cuir Noir + Ceinture Simili Cuir Noire</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2 450 FCFA</t>
+          <t>4 000 FCFA</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Jean Fin Ample Pour Homme, Pantalon De Travail élastique, Coupe Droite, Lavage, Décontracté</t>
+          <t>Ensemble Djalaba pour homme - Djelaba + pantalon</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
       <c r="C64" t="inlineStr">
         <is>
-          <t>3 400 FCFA</t>
+          <t>9 999 FCFA</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2 en 1 Short à manches courtes pour homme Ensemble décontracté-Blanc</t>
+          <t>Sac de ceinture étanche en toile banane pour course à pied, Sport, Jogging, Portable, extérieur, ceinture, femmes, hommes, accessoires de Sport</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr">
         <is>
-          <t>3 200 FCFA</t>
+          <t>3 600 FCFA - 4 080 FCFA</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Chaussures De Travail En Cuir à Lacets Pour Hommes</t>
+          <t>Lunettes  photogray anti reflet - Unisex - motif Guépard</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr">
         <is>
-          <t>5 200 FCFA - 7 353 FCFA</t>
+          <t>5 500 FCFA</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Baskets Décontractées Pour Hommes</t>
+          <t>chapelet de priéré multicolres</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr">
         <is>
-          <t>8 600 FCFA</t>
+          <t>4 999 FCFA</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Chaussures Formelles élégantes à Bout Pointu Pour Hommes</t>
+          <t>Ensemble Djalaba pour homme - Djelaba + pantalon</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr">
         <is>
-          <t>5 900 FCFA - 7 900 FCFA</t>
+          <t>9 999 FCFA</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Jeans En Denim à La Mode Pour Hommes - 2pc - Beige Bleu</t>
+          <t>Robe simple -  100% coton - Confortable - Adaptée à votre corps</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr">
         <is>
-          <t>6 800 FCFA</t>
+          <t>10 999 FCFA</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Montre d'affaires étanche à double calendrier - Argent et or</t>
+          <t>Coffret de priére de 6pcs - tapis de priere- parfum - Djalaba - chapelet - stylo - livre CORAN</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr">
         <is>
-          <t>3 900 FCFA</t>
+          <t>16 900 FCFA</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Chaussures Habillées Pour Hommes</t>
+          <t>Lot de 5 T-shirts de couleurs différentes .</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr">
         <is>
-          <t>3 460 FCFA - 5 900 FCFA</t>
+          <t>9 994 FCFA</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Chaussons Des Sandales Femme</t>
+          <t>Coffret de priére de 6pcs - tapis de priere- parfum - Djalaba - chapelet - stylo - livre citadelle du musulmane</t>
         </is>
       </c>
       <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr">
         <is>
-          <t>1 905 FCFA</t>
+          <t>16 900 FCFA</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Chemise Manches Longues Pour Homme</t>
+          <t>Ensemble robe + foulard pudique et confortable - conton Bleu</t>
         </is>
       </c>
       <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr">
         <is>
-          <t>2 205 FCFA</t>
+          <t>7 200 FCFA</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Montre A Quartz Pour Femme - Or</t>
+          <t>Chaussures homme basket Chaussures décontractées pour hommes</t>
         </is>
       </c>
       <c r="B74" t="inlineStr"/>
       <c r="C74" t="inlineStr">
         <is>
-          <t>1 450 FCFA</t>
+          <t>6 800 FCFA</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Chaussures décontractées à talons en toile pour hommes</t>
+          <t>Bottes de désert montantes pour hommes en plein air</t>
         </is>
       </c>
       <c r="B75" t="inlineStr"/>
       <c r="C75" t="inlineStr">
         <is>
-          <t>2 250 FCFA</t>
+          <t>9 900 FCFA</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Robe Assortie Imprimée-vert</t>
+          <t>Casquette de mode - Bleu de nuit</t>
         </is>
       </c>
       <c r="B76" t="inlineStr"/>
       <c r="C76" t="inlineStr">
         <is>
-          <t>2 320 FCFA</t>
+          <t>2 400 FCFA</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Chemise Hawaïenne Homme - multicolore</t>
+          <t>Nouvelles chaussures de sport respirantes pour hommes</t>
         </is>
       </c>
       <c r="B77" t="inlineStr"/>
       <c r="C77" t="inlineStr">
         <is>
-          <t>1 855 FCFA - 3 790 FCFA</t>
+          <t>6 300 FCFA</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Chemise Homme Manches Longues Décontracté-Bleu</t>
+          <t>Chaussures En Cuir Pour Hommes, Chaussures Décontractées, Flexion Arbitraire+Chaussettes (cadeau)</t>
         </is>
       </c>
       <c r="B78" t="inlineStr"/>
       <c r="C78" t="inlineStr">
         <is>
-          <t>1 810 FCFA</t>
+          <t>4 125 FCFA</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Baskets Mode Homme + chaussettes</t>
+          <t>Ensemble COLIER ET BOUCLE D'OREILLES</t>
         </is>
       </c>
       <c r="B79" t="inlineStr"/>
       <c r="C79" t="inlineStr">
         <is>
-          <t>5 900 FCFA</t>
+          <t>2 720 FCFA</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Polo Court Homme - gris</t>
+          <t>Casquette de mode Noir</t>
         </is>
       </c>
       <c r="B80" t="inlineStr"/>
       <c r="C80" t="inlineStr">
         <is>
-          <t>4 580 FCFA</t>
+          <t>2 240 FCFA</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Nouvelles chaussures de sport respirantes pour hommes - Blanc</t>
+          <t>Jallabe - Manches longues - avec capuchon Homme</t>
         </is>
       </c>
       <c r="B81" t="inlineStr"/>
       <c r="C81" t="inlineStr">
         <is>
-          <t>2 400 FCFA</t>
+          <t>10 200 FCFA</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Pantalons Décontractés Pour Hommes</t>
+          <t>2 Piece Short -sleeved Shirt Mens Soprtswear Trousers Pants</t>
         </is>
       </c>
       <c r="B82" t="inlineStr"/>
       <c r="C82" t="inlineStr">
         <is>
-          <t>2 130 FCFA</t>
+          <t>5 200 FCFA</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Ballerines Class Pour Femme - Noir</t>
+          <t>Baskets Décontractées Pour Hommes + chaussette</t>
         </is>
       </c>
       <c r="B83" t="inlineStr"/>
       <c r="C83" t="inlineStr">
         <is>
-          <t>1 810 FCFA</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>Bottes de désert montantes pour hommes en plein air</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr"/>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>8 900 FCFA - 9 900 FCFA</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>Chaussures en Toile Homme + Ceinture Noir</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr"/>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>2 500 FCFA</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>Chaussures Décontractées Pour Hommes + ceinture</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr"/>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>3 500 FCFA</t>
+          <t>4 300 FCFA</t>
         </is>
       </c>
     </row>

</xml_diff>